<commit_message>
small changes by kiran
</commit_message>
<xml_diff>
--- a/mini_project2/Excel/Data.xlsx
+++ b/mini_project2/Excel/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiran\eclipse-workspace\mini_project2\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiran\git\mini_project2\mini_project2\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9214DA16-A0F3-42C4-9417-B843139ABB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC27F91-2A9E-4949-B00C-BC23AB566C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="2460" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,10 +37,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -63,13 +71,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -351,7 +362,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -361,14 +372,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{5349A326-B2F9-4F8D-B702-E4F90DA9801D}"/>
+    <hyperlink ref="B1" r:id="rId2" xr:uid="{2E2EE85F-BA36-451A-AC74-834FBF507F5E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>